<commit_message>
added a few text edits
</commit_message>
<xml_diff>
--- a/Qualitative_work/Qualitative_consultations/2_Data_raw/Data_Qualitative consultations_raw.xlsx
+++ b/Qualitative_work/Qualitative_consultations/2_Data_raw/Data_Qualitative consultations_raw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgiar-my.sharepoint.com/personal/l_nabwire_cgiar_org/Documents/Documents/mippi_UG_forked/Qualitative_work/Qualitative_consultations/2_Data_raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgiar-my.sharepoint.com/personal/l_nabwire_cgiar_org/Documents/L.Nabwire/git/Maize_Uganda/mippi_UG/Qualitative_work/Qualitative_consultations/2_Data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{E0445B33-EB7F-402F-ABBB-1224E72B093B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA8F3573-2380-48C5-991F-AF7FEED714C5}"/>
+  <xr:revisionPtr revIDLastSave="411" documentId="8_{E0445B33-EB7F-402F-ABBB-1224E72B093B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5036B18-57F5-4E1A-BD5A-6F52D6470F40}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="q1" sheetId="14" r:id="rId1"/>
@@ -23,8 +23,17 @@
     <sheet name="7a" sheetId="23" r:id="rId8"/>
     <sheet name="q8" sheetId="31" r:id="rId9"/>
     <sheet name="q9" sheetId="32" r:id="rId10"/>
+    <sheet name="q1_p" sheetId="33" r:id="rId11"/>
+    <sheet name="q2_p" sheetId="34" r:id="rId12"/>
+    <sheet name="q3_p" sheetId="35" r:id="rId13"/>
+    <sheet name="q3a_p" sheetId="36" r:id="rId14"/>
+    <sheet name="q4_p" sheetId="37" r:id="rId15"/>
+    <sheet name="q5_p" sheetId="38" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="6" r:id="rId17"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -42,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="262">
   <si>
     <t>Aroma</t>
   </si>
@@ -585,13 +594,256 @@
   </si>
   <si>
     <t>Fine flour texture</t>
+  </si>
+  <si>
+    <t>Men</t>
+  </si>
+  <si>
+    <t>Women</t>
+  </si>
+  <si>
+    <t>Longe 4</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Variety</t>
+  </si>
+  <si>
+    <t>Variety prefereces by sex</t>
+  </si>
+  <si>
+    <t>who makes decisions to adopt/change to a new maize variety, and why</t>
+  </si>
+  <si>
+    <t>who</t>
+  </si>
+  <si>
+    <t>why</t>
+  </si>
+  <si>
+    <t>men</t>
+  </si>
+  <si>
+    <t>he is the head of the family</t>
+  </si>
+  <si>
+    <t>who makes decisions on what maize variety to grow, and why</t>
+  </si>
+  <si>
+    <t>because they are responsibe for all plans at home</t>
+  </si>
+  <si>
+    <t>Do the household members that decide which crops to grow also have a role in preparing the food?</t>
+  </si>
+  <si>
+    <t>yes/no</t>
+  </si>
+  <si>
+    <t>Traders &amp; farmers</t>
+  </si>
+  <si>
+    <t>Barriers to adoption by gender</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>barrier</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Ignorance/information gap</t>
+  </si>
+  <si>
+    <t>Climate change</t>
+  </si>
+  <si>
+    <t>Inaccability to land</t>
+  </si>
+  <si>
+    <t>Poor decision making</t>
+  </si>
+  <si>
+    <t>Youth</t>
+  </si>
+  <si>
+    <t>Limited funds</t>
+  </si>
+  <si>
+    <t>Group influence</t>
+  </si>
+  <si>
+    <t>Incentives to adoption by sex</t>
+  </si>
+  <si>
+    <t>incentive</t>
+  </si>
+  <si>
+    <t>Subsidizing the price of seed</t>
+  </si>
+  <si>
+    <t>Access to affordable loans</t>
+  </si>
+  <si>
+    <t>Access to land</t>
+  </si>
+  <si>
+    <t>Early maturing varieties</t>
+  </si>
+  <si>
+    <t>High yielding varieties</t>
+  </si>
+  <si>
+    <t>Information/training about new maize varieties</t>
+  </si>
+  <si>
+    <t>Crop insurance</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>men and youth</t>
+  </si>
+  <si>
+    <t>women &amp; youth</t>
+  </si>
+  <si>
+    <t>Early maturing</t>
+  </si>
+  <si>
+    <t>It is his duty</t>
+  </si>
+  <si>
+    <t>Millers &amp; seed dealers</t>
+  </si>
+  <si>
+    <t>they own land</t>
+  </si>
+  <si>
+    <t>they are the decision makers</t>
+  </si>
+  <si>
+    <t>women have movemeny limitations (they spend more time in the gardens)</t>
+  </si>
+  <si>
+    <t>they are more financially stable</t>
+  </si>
+  <si>
+    <t>they spend more time in the urban centers where agro-shops are found.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lack of information and communication </t>
+  </si>
+  <si>
+    <t>Lack of ownership of land</t>
+  </si>
+  <si>
+    <t>Women are not involved in decision making</t>
+  </si>
+  <si>
+    <t>barrier theme</t>
+  </si>
+  <si>
+    <t>Gender based violence</t>
+  </si>
+  <si>
+    <t>Low finances to buy seed and other inputs.</t>
+  </si>
+  <si>
+    <t>Lack of funds to buy seed</t>
+  </si>
+  <si>
+    <t>Limited access to land</t>
+  </si>
+  <si>
+    <t>free inputs for trial</t>
+  </si>
+  <si>
+    <t>market availability</t>
+  </si>
+  <si>
+    <t>extension services and training</t>
+  </si>
+  <si>
+    <t>Demonstrations/trial gardens</t>
+  </si>
+  <si>
+    <t>women</t>
+  </si>
+  <si>
+    <t>youth</t>
+  </si>
+  <si>
+    <t>to ensure household food security</t>
+  </si>
+  <si>
+    <t>they know the high yielding varieties</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Lack of finance</t>
+  </si>
+  <si>
+    <t>No land rights</t>
+  </si>
+  <si>
+    <t>land of land ownership</t>
+  </si>
+  <si>
+    <t>food security</t>
+  </si>
+  <si>
+    <t>Proportion of responses</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Sum of Proportion of responses</t>
+  </si>
+  <si>
+    <t>No. of respodents in the group</t>
+  </si>
+  <si>
+    <t>Nutritious</t>
+  </si>
+  <si>
+    <t>cost of seed</t>
+  </si>
+  <si>
+    <t>limited awareness</t>
+  </si>
+  <si>
+    <t>unpredictable weather</t>
+  </si>
+  <si>
+    <t>Limited decision making</t>
+  </si>
+  <si>
+    <t>Poor attidute</t>
+  </si>
+  <si>
+    <t>Poot attitude</t>
+  </si>
+  <si>
+    <t>gender based violence</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -757,6 +1009,20 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1109,7 +1375,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1160,6 +1426,14 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1223,6 +1497,458 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Administrator" refreshedDate="45182.627585532406" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="47" xr:uid="{6ACB03FA-4469-46ED-AEEA-C9059F71CA7C}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="B3:E50" sheet="q1"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="Attribute category" numFmtId="0">
+      <sharedItems count="3">
+        <s v="Production"/>
+        <s v="Consumption"/>
+        <s v="Production &amp; consumption"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="attribute" numFmtId="0">
+      <sharedItems count="14">
+        <s v="Yield"/>
+        <s v="Drought tolerace"/>
+        <s v="Grain size/weight"/>
+        <s v="Quality of flour (color &amp; texture)"/>
+        <s v="Milling out-turn"/>
+        <s v="Pest &amp; disease tolerance"/>
+        <s v="Maturity time"/>
+        <s v="Palatability (sweet &amp; smooth taste)"/>
+        <s v="Shelf life"/>
+        <s v="Recycling potential"/>
+        <s v="Nutrition/protein"/>
+        <s v="Flour expansion after cooking"/>
+        <s v="Reqires less inputs"/>
+        <s v="Cost of seed"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Number of respondents in the group" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="4"/>
+    </cacheField>
+    <cacheField name="Proportion of responses" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.282051282051282E-2" maxValue="2.564102564102564E-2"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="47">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="3"/>
+    <n v="1.9230769230769232E-2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="3"/>
+    <n v="1.9230769230769232E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="1.9230769230769232E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="4"/>
+    <n v="2.564102564102564E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="4"/>
+    <n v="2.564102564102564E-2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="2.564102564102564E-2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="4"/>
+    <n v="2.564102564102564E-2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="4"/>
+    <n v="2.564102564102564E-2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="6"/>
+    <n v="4"/>
+    <n v="2.564102564102564E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <n v="4"/>
+    <n v="2.564102564102564E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <n v="4"/>
+    <n v="2.564102564102564E-2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="6"/>
+    <n v="4"/>
+    <n v="2.564102564102564E-2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="2.564102564102564E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="4"/>
+    <n v="2.564102564102564E-2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="4"/>
+    <n v="2.564102564102564E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="3"/>
+    <n v="1.9230769230769232E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="1.9230769230769232E-2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="6"/>
+    <n v="3"/>
+    <n v="1.9230769230769232E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <n v="3"/>
+    <n v="1.9230769230769232E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="3"/>
+    <n v="1.9230769230769232E-2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="2"/>
+    <n v="1.282051282051282E-2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="6"/>
+    <n v="2"/>
+    <n v="1.282051282051282E-2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="2"/>
+    <n v="1.282051282051282E-2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="9"/>
+    <n v="2"/>
+    <n v="1.282051282051282E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="2"/>
+    <n v="1.282051282051282E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <n v="2"/>
+    <n v="1.282051282051282E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <n v="2"/>
+    <n v="1.282051282051282E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <n v="2"/>
+    <n v="1.282051282051282E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="11"/>
+    <n v="2"/>
+    <n v="1.282051282051282E-2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="6"/>
+    <n v="4"/>
+    <n v="2.564102564102564E-2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="2.564102564102564E-2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="4"/>
+    <n v="2.564102564102564E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="4"/>
+    <n v="2.564102564102564E-2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="12"/>
+    <n v="4"/>
+    <n v="2.564102564102564E-2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="2.564102564102564E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="4"/>
+    <n v="2.564102564102564E-2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="12"/>
+    <n v="4"/>
+    <n v="2.564102564102564E-2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="4"/>
+    <n v="2.564102564102564E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <n v="4"/>
+    <n v="2.564102564102564E-2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="13"/>
+    <n v="4"/>
+    <n v="2.564102564102564E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="4"/>
+    <n v="2.564102564102564E-2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="3"/>
+    <n v="1.9230769230769232E-2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="3"/>
+    <n v="1.9230769230769232E-2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="13"/>
+    <n v="3"/>
+    <n v="1.9230769230769232E-2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="6"/>
+    <n v="3"/>
+    <n v="1.9230769230769232E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <n v="3"/>
+    <n v="1.9230769230769232E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="3"/>
+    <n v="1.9230769230769232E-2"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D380E609-A27E-4E90-A175-D9B3BE1E36D9}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="G4:H23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="15">
+        <item x="13"/>
+        <item x="1"/>
+        <item x="11"/>
+        <item x="2"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="10"/>
+        <item x="7"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item x="9"/>
+        <item x="12"/>
+        <item x="8"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="0"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="19">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Proportion of responses" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1524,11 +2250,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1537,6 +2263,8 @@
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="19.08984375" customWidth="1"/>
     <col min="4" max="4" width="11.7265625" customWidth="1"/>
+    <col min="7" max="7" width="34" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -1546,16 +2274,14 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="15"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:8" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>23</v>
       </c>
@@ -1568,9 +2294,11 @@
       <c r="D3" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="E3" s="4" t="s">
+        <v>249</v>
+      </c>
       <c r="F3"/>
       <c r="G3"/>
-      <c r="H3"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -1585,6 +2313,16 @@
       <c r="D4">
         <v>3</v>
       </c>
+      <c r="E4">
+        <f>D4/$D$51</f>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="H4" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -1599,6 +2337,16 @@
       <c r="D5">
         <v>3</v>
       </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E50" si="0">D5/$D$51</f>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5">
+        <v>0.42948717948717952</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -1613,6 +2361,16 @@
       <c r="D6">
         <v>3</v>
       </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6">
+        <v>1.282051282051282E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -1627,6 +2385,16 @@
       <c r="D7">
         <v>4</v>
       </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="H7">
+        <v>0.11538461538461536</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -1641,6 +2409,16 @@
       <c r="D8">
         <v>4</v>
       </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8">
+        <v>2.564102564102564E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -1655,6 +2433,16 @@
       <c r="D9">
         <v>4</v>
       </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9">
+        <v>0.10256410256410257</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -1669,6 +2457,16 @@
       <c r="D10">
         <v>4</v>
       </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10">
+        <v>1.282051282051282E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -1683,6 +2481,16 @@
       <c r="D11">
         <v>4</v>
       </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11">
+        <v>7.6923076923076927E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -1697,6 +2505,16 @@
       <c r="D12">
         <v>4</v>
       </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12">
+        <v>4.4871794871794872E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -1711,6 +2529,16 @@
       <c r="D13">
         <v>4</v>
       </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+      <c r="G13" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13">
+        <v>3.8461538461538464E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -1725,6 +2553,16 @@
       <c r="D14">
         <v>4</v>
       </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14">
+        <v>0.44230769230769229</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -1739,6 +2577,16 @@
       <c r="D15">
         <v>4</v>
       </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15">
+        <v>4.4871794871794872E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -1753,8 +2601,18 @@
       <c r="D16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16">
+        <v>0.10897435897435898</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1767,8 +2625,18 @@
       <c r="D17">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+      <c r="G17" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1781,8 +2649,18 @@
       <c r="D18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+      <c r="G18" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18">
+        <v>1.282051282051282E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1795,8 +2673,18 @@
       <c r="D19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19">
+        <v>5.128205128205128E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -1809,8 +2697,18 @@
       <c r="D20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20">
+        <v>0.14102564102564102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1823,8 +2721,18 @@
       <c r="D21">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21">
+        <v>0.12820512820512819</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1837,8 +2745,18 @@
       <c r="D22">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22">
+        <v>0.12820512820512819</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -1851,8 +2769,18 @@
       <c r="D23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>251</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -1865,8 +2793,12 @@
       <c r="D24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>1.282051282051282E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -1879,8 +2811,12 @@
       <c r="D25">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>1.282051282051282E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -1893,8 +2829,12 @@
       <c r="D26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>1.282051282051282E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -1907,8 +2847,12 @@
       <c r="D27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>1.282051282051282E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1921,8 +2865,12 @@
       <c r="D28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>1.282051282051282E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1935,8 +2883,12 @@
       <c r="D29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>1.282051282051282E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -1949,8 +2901,12 @@
       <c r="D30">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>1.282051282051282E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -1963,8 +2919,12 @@
       <c r="D31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>1.282051282051282E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -1977,8 +2937,12 @@
       <c r="D32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>1.282051282051282E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -1991,8 +2955,12 @@
       <c r="D33">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -2005,8 +2973,12 @@
       <c r="D34">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -2019,8 +2991,12 @@
       <c r="D35">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -2033,8 +3009,12 @@
       <c r="D36">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -2047,8 +3027,12 @@
       <c r="D37">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -2061,8 +3045,12 @@
       <c r="D38">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -2075,8 +3063,12 @@
       <c r="D39">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -2089,8 +3081,12 @@
       <c r="D40">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -2103,8 +3099,12 @@
       <c r="D41">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -2117,8 +3117,12 @@
       <c r="D42">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -2131,8 +3135,12 @@
       <c r="D43">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -2145,8 +3153,12 @@
       <c r="D44">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -2159,8 +3171,12 @@
       <c r="D45">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -2173,8 +3189,12 @@
       <c r="D46">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>43</v>
       </c>
@@ -2187,8 +3207,12 @@
       <c r="D47">
         <v>3</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>43</v>
       </c>
@@ -2201,8 +3225,12 @@
       <c r="D48">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>43</v>
       </c>
@@ -2215,8 +3243,12 @@
       <c r="D49">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E49">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>43</v>
       </c>
@@ -2229,8 +3261,12 @@
       <c r="D50">
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E50">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D51">
         <f>SUM(D4:D50)</f>
         <v>156</v>
@@ -2238,7 +3274,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2421,6 +3457,1122 @@
       <c r="D14">
         <f>SUM(D4:D13)</f>
         <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94A15736-EDFA-4DE1-9CE7-23CD6F8E3720}">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>196</v>
+      </c>
+      <c r="B6" t="s">
+        <v>219</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>222</v>
+      </c>
+      <c r="B7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>254</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>217</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>222</v>
+      </c>
+      <c r="B9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>222</v>
+      </c>
+      <c r="B10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>165</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>222</v>
+      </c>
+      <c r="B11" t="s">
+        <v>205</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>217</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>222</v>
+      </c>
+      <c r="B12" t="s">
+        <v>219</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>217</v>
+      </c>
+      <c r="E12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>222</v>
+      </c>
+      <c r="B13" t="s">
+        <v>218</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>220</v>
+      </c>
+      <c r="E13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" t="s">
+        <v>240</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>254</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" t="s">
+        <v>240</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>220</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" t="s">
+        <v>190</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>165</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" t="s">
+        <v>190</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>165</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" t="s">
+        <v>241</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>220</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" t="s">
+        <v>205</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>220</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E20">
+        <f>SUM(E3:E19)</f>
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="24" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864F6554-710E-4A52-BA13-CA3511896B2E}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>222</v>
+      </c>
+      <c r="B7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA23668-79A0-4795-82E7-42EB00A52C9F}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8591E64-C7FC-48CD-9C9D-9C702E1E928D}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{101BA3BC-630A-4927-964A-A8026DFE6ECB}">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.453125" customWidth="1"/>
+    <col min="3" max="3" width="37.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" t="s">
+        <v>201</v>
+      </c>
+      <c r="D4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>196</v>
+      </c>
+      <c r="B6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>196</v>
+      </c>
+      <c r="B7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C7" t="s">
+        <v>204</v>
+      </c>
+      <c r="D7" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B8" t="s">
+        <v>205</v>
+      </c>
+      <c r="C8" t="s">
+        <v>206</v>
+      </c>
+      <c r="D8" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C9" t="s">
+        <v>259</v>
+      </c>
+      <c r="D9" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C10" t="s">
+        <v>207</v>
+      </c>
+      <c r="D10" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>222</v>
+      </c>
+      <c r="B11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C11" t="s">
+        <v>228</v>
+      </c>
+      <c r="D11" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>222</v>
+      </c>
+      <c r="B12" t="s">
+        <v>181</v>
+      </c>
+      <c r="C12" t="s">
+        <v>233</v>
+      </c>
+      <c r="D12" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>222</v>
+      </c>
+      <c r="B13" t="s">
+        <v>182</v>
+      </c>
+      <c r="C13" t="s">
+        <v>229</v>
+      </c>
+      <c r="D13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>222</v>
+      </c>
+      <c r="B14" t="s">
+        <v>182</v>
+      </c>
+      <c r="C14" t="s">
+        <v>230</v>
+      </c>
+      <c r="D14" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>222</v>
+      </c>
+      <c r="B15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C15" t="s">
+        <v>232</v>
+      </c>
+      <c r="D15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>222</v>
+      </c>
+      <c r="B16" t="s">
+        <v>205</v>
+      </c>
+      <c r="C16" t="s">
+        <v>234</v>
+      </c>
+      <c r="D16" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>222</v>
+      </c>
+      <c r="B17" t="s">
+        <v>205</v>
+      </c>
+      <c r="C17" t="s">
+        <v>235</v>
+      </c>
+      <c r="D17" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" t="s">
+        <v>190</v>
+      </c>
+      <c r="C18" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" t="s">
+        <v>182</v>
+      </c>
+      <c r="C19" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" t="s">
+        <v>205</v>
+      </c>
+      <c r="C20" t="s">
+        <v>247</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94095180-4E71-4210-9243-63581AEE253E}">
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>196</v>
+      </c>
+      <c r="B6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>196</v>
+      </c>
+      <c r="B7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C10" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B11" t="s">
+        <v>205</v>
+      </c>
+      <c r="C11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>222</v>
+      </c>
+      <c r="B12" t="s">
+        <v>181</v>
+      </c>
+      <c r="C12" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>222</v>
+      </c>
+      <c r="B13" t="s">
+        <v>181</v>
+      </c>
+      <c r="C13" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>222</v>
+      </c>
+      <c r="B14" t="s">
+        <v>182</v>
+      </c>
+      <c r="C14" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>222</v>
+      </c>
+      <c r="B15" t="s">
+        <v>205</v>
+      </c>
+      <c r="C15" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" t="s">
+        <v>181</v>
+      </c>
+      <c r="C16" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" t="s">
+        <v>190</v>
+      </c>
+      <c r="C17" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" t="s">
+        <v>190</v>
+      </c>
+      <c r="C18" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" t="s">
+        <v>240</v>
+      </c>
+      <c r="C19" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" t="s">
+        <v>240</v>
+      </c>
+      <c r="C20" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" t="s">
+        <v>240</v>
+      </c>
+      <c r="C21" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>110</v>
+      </c>
+      <c r="B22" t="s">
+        <v>205</v>
+      </c>
+      <c r="C22" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" t="s">
+        <v>205</v>
+      </c>
+      <c r="C23" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -2449,11 +4601,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
       <c r="E1" s="16" t="s">
         <v>83</v>
       </c>
@@ -3462,13 +5614,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
       <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -3742,7 +5894,7 @@
   <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
@@ -3757,12 +5909,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:6" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">

</xml_diff>